<commit_message>
Update Copy of Messy Data Sample .xlsx
</commit_message>
<xml_diff>
--- a/Copy of Messy Data Sample .xlsx
+++ b/Copy of Messy Data Sample .xlsx
@@ -8,35 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\GitHub\my_qa_repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4FB62262-496E-4DBD-9600-AC445DB39C7A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0441BB22-35A7-48CD-A18C-8A581ED62BDC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29070" yWindow="645" windowWidth="27870" windowHeight="14505" xr2:uid="{65D4A02A-0F20-4F9E-972B-23CE08E7D936}"/>
   </bookViews>
   <sheets>
     <sheet name="Messy Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Tidy Version 1" sheetId="2" r:id="rId2"/>
+    <sheet name="Tidy Version 2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="81">
   <si>
     <t>Sunderland, UK</t>
   </si>
@@ -144,16 +135,204 @@
   </si>
   <si>
     <t>Twenty two</t>
+  </si>
+  <si>
+    <t>Town/City</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>UK</t>
+  </si>
+  <si>
+    <t>Leeds</t>
+  </si>
+  <si>
+    <t>Sunderland</t>
+  </si>
+  <si>
+    <t>Warrington</t>
+  </si>
+  <si>
+    <t>Dover</t>
+  </si>
+  <si>
+    <t>Manchester</t>
+  </si>
+  <si>
+    <t>Sheffield</t>
+  </si>
+  <si>
+    <t>Huddersfield</t>
+  </si>
+  <si>
+    <t>Leicester</t>
+  </si>
+  <si>
+    <t>Birmingham</t>
+  </si>
+  <si>
+    <t>Felixstowe</t>
+  </si>
+  <si>
+    <t>London</t>
+  </si>
+  <si>
+    <t>Cardiff</t>
+  </si>
+  <si>
+    <t>Glasgow</t>
+  </si>
+  <si>
+    <t>Belfast</t>
+  </si>
+  <si>
+    <t>Insert new row to allow for Headers - Town/City, Country</t>
+  </si>
+  <si>
+    <r>
+      <t>Removed all instances of '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, UK</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' in the Town/City column</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Amended UK, Leeds to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Leeds</t>
+    </r>
+  </si>
+  <si>
+    <t>A10</t>
+  </si>
+  <si>
+    <t>A13</t>
+  </si>
+  <si>
+    <t>Dudley</t>
+  </si>
+  <si>
+    <r>
+      <t>Deleted</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> , United Kingdom</t>
+    </r>
+  </si>
+  <si>
+    <t>A6 &amp; A18</t>
+  </si>
+  <si>
+    <t>Used Conditional Formatting to ensure rows were duplicates</t>
+  </si>
+  <si>
+    <t>A18</t>
+  </si>
+  <si>
+    <t>Deleted row 18</t>
+  </si>
+  <si>
+    <t>A8 &amp; A17</t>
+  </si>
+  <si>
+    <t>Same as above</t>
+  </si>
+  <si>
+    <t>A17</t>
+  </si>
+  <si>
+    <t>Deleted row 17</t>
+  </si>
+  <si>
+    <t>Column F</t>
+  </si>
+  <si>
+    <t>Inserted column and named it 2016</t>
+  </si>
+  <si>
+    <t>G10</t>
+  </si>
+  <si>
+    <t>Converted text to number</t>
+  </si>
+  <si>
+    <t>Column I</t>
+  </si>
+  <si>
+    <t>Created new column to the left to allow for transposition of data from Column H representing 2019</t>
+  </si>
+  <si>
+    <t>Transposed numerical data from column H representing 2019</t>
+  </si>
+  <si>
+    <t>A16</t>
+  </si>
+  <si>
+    <t>Corrected spelling for Middlesbrough</t>
+  </si>
+  <si>
+    <t>Middlesbrough</t>
+  </si>
+  <si>
+    <t>Column K</t>
+  </si>
+  <si>
+    <t>Renamed 2021</t>
+  </si>
+  <si>
+    <t>Completed borders for all fields</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -173,7 +352,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -196,19 +375,133 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{9FE0147B-50EC-433E-96D4-28015926AC66}"/>
   </tableStyles>
@@ -522,7 +815,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22F17CA9-555E-46BA-8B48-FA77E17B919F}">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1112,4 +1407,1514 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9055D27-0F79-4197-BEB9-548CFED8AF71}">
+  <dimension ref="A1:O19"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:O19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2">
+        <v>2013</v>
+      </c>
+      <c r="D2" s="2">
+        <v>2014</v>
+      </c>
+      <c r="E2" s="2">
+        <v>2015</v>
+      </c>
+      <c r="F2" s="2">
+        <v>2016</v>
+      </c>
+      <c r="G2" s="2">
+        <v>2017</v>
+      </c>
+      <c r="H2" s="2">
+        <v>2018</v>
+      </c>
+      <c r="I2" s="2">
+        <v>2019</v>
+      </c>
+      <c r="J2" s="2">
+        <v>2020</v>
+      </c>
+      <c r="K2" s="2">
+        <v>2021</v>
+      </c>
+      <c r="L2" s="2">
+        <v>2022</v>
+      </c>
+      <c r="O2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="1">
+        <v>28</v>
+      </c>
+      <c r="D3" s="1">
+        <v>27</v>
+      </c>
+      <c r="E3" s="1">
+        <v>24</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1">
+        <v>21</v>
+      </c>
+      <c r="H3" s="1">
+        <v>17</v>
+      </c>
+      <c r="I3" s="1">
+        <v>19</v>
+      </c>
+      <c r="J3" s="1">
+        <v>18</v>
+      </c>
+      <c r="K3" s="1">
+        <v>20</v>
+      </c>
+      <c r="L3" s="1">
+        <v>20</v>
+      </c>
+      <c r="O3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="1">
+        <v>48</v>
+      </c>
+      <c r="D4" s="1">
+        <v>51</v>
+      </c>
+      <c r="E4" s="1">
+        <v>47</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1">
+        <v>52</v>
+      </c>
+      <c r="H4" s="1">
+        <v>39</v>
+      </c>
+      <c r="I4" s="1">
+        <v>43</v>
+      </c>
+      <c r="J4" s="1">
+        <v>42</v>
+      </c>
+      <c r="K4" s="1">
+        <v>47</v>
+      </c>
+      <c r="L4" s="1">
+        <v>37</v>
+      </c>
+      <c r="N4" t="s">
+        <v>56</v>
+      </c>
+      <c r="O4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="1">
+        <v>60</v>
+      </c>
+      <c r="D5" s="1">
+        <v>72</v>
+      </c>
+      <c r="E5" s="1">
+        <v>54</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1">
+        <v>66</v>
+      </c>
+      <c r="H5" s="1">
+        <v>45</v>
+      </c>
+      <c r="I5" s="1">
+        <v>48</v>
+      </c>
+      <c r="J5" s="1">
+        <v>49</v>
+      </c>
+      <c r="K5" s="1">
+        <v>55</v>
+      </c>
+      <c r="L5" s="1">
+        <v>49</v>
+      </c>
+      <c r="N5" t="s">
+        <v>57</v>
+      </c>
+      <c r="O5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="1">
+        <v>25</v>
+      </c>
+      <c r="D6" s="1">
+        <v>34</v>
+      </c>
+      <c r="E6" s="1">
+        <v>39</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1">
+        <v>34</v>
+      </c>
+      <c r="H6" s="1">
+        <v>29</v>
+      </c>
+      <c r="I6" s="1">
+        <v>28</v>
+      </c>
+      <c r="J6" s="1">
+        <v>34</v>
+      </c>
+      <c r="K6" s="1">
+        <v>48</v>
+      </c>
+      <c r="L6" s="1">
+        <v>37</v>
+      </c>
+      <c r="N6" t="s">
+        <v>60</v>
+      </c>
+      <c r="O6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="1">
+        <v>115</v>
+      </c>
+      <c r="D7" s="1">
+        <v>104</v>
+      </c>
+      <c r="E7" s="1">
+        <v>115</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1">
+        <v>119</v>
+      </c>
+      <c r="H7" s="1">
+        <v>95</v>
+      </c>
+      <c r="I7" s="1">
+        <v>99</v>
+      </c>
+      <c r="J7" s="1">
+        <v>98</v>
+      </c>
+      <c r="K7" s="1">
+        <v>88</v>
+      </c>
+      <c r="L7" s="1">
+        <v>78</v>
+      </c>
+      <c r="N7" t="s">
+        <v>62</v>
+      </c>
+      <c r="O7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="1">
+        <v>52</v>
+      </c>
+      <c r="D8" s="1">
+        <v>42</v>
+      </c>
+      <c r="E8" s="1">
+        <v>37</v>
+      </c>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1">
+        <v>38</v>
+      </c>
+      <c r="H8" s="1">
+        <v>25</v>
+      </c>
+      <c r="I8" s="1">
+        <v>34</v>
+      </c>
+      <c r="J8" s="1">
+        <v>35</v>
+      </c>
+      <c r="K8" s="1">
+        <v>32</v>
+      </c>
+      <c r="L8" s="1">
+        <v>39</v>
+      </c>
+      <c r="N8" t="s">
+        <v>64</v>
+      </c>
+      <c r="O8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="1">
+        <v>70</v>
+      </c>
+      <c r="D9" s="1">
+        <v>60</v>
+      </c>
+      <c r="E9" s="1">
+        <v>63</v>
+      </c>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1">
+        <v>51</v>
+      </c>
+      <c r="H9" s="1">
+        <v>46</v>
+      </c>
+      <c r="I9" s="1">
+        <v>53</v>
+      </c>
+      <c r="J9" s="1">
+        <v>46</v>
+      </c>
+      <c r="K9" s="1">
+        <v>51</v>
+      </c>
+      <c r="L9" s="1">
+        <v>66</v>
+      </c>
+      <c r="N9" t="s">
+        <v>66</v>
+      </c>
+      <c r="O9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="1">
+        <v>98</v>
+      </c>
+      <c r="D10" s="1">
+        <v>92</v>
+      </c>
+      <c r="E10" s="1">
+        <v>104</v>
+      </c>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1">
+        <v>22</v>
+      </c>
+      <c r="H10" s="1">
+        <v>81</v>
+      </c>
+      <c r="I10" s="1">
+        <v>77</v>
+      </c>
+      <c r="J10" s="1">
+        <v>87</v>
+      </c>
+      <c r="K10" s="1">
+        <v>101</v>
+      </c>
+      <c r="L10" s="1">
+        <v>87</v>
+      </c>
+      <c r="N10" t="s">
+        <v>68</v>
+      </c>
+      <c r="O10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="1">
+        <v>172</v>
+      </c>
+      <c r="D11" s="1">
+        <v>179</v>
+      </c>
+      <c r="E11" s="1">
+        <v>192</v>
+      </c>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1">
+        <v>182</v>
+      </c>
+      <c r="H11" s="1">
+        <v>154</v>
+      </c>
+      <c r="I11" s="1">
+        <v>212</v>
+      </c>
+      <c r="J11" s="1">
+        <v>173</v>
+      </c>
+      <c r="K11" s="1">
+        <v>172</v>
+      </c>
+      <c r="L11" s="1">
+        <v>167</v>
+      </c>
+      <c r="N11" t="s">
+        <v>70</v>
+      </c>
+      <c r="O11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="1">
+        <v>233</v>
+      </c>
+      <c r="D12" s="1">
+        <v>229</v>
+      </c>
+      <c r="E12" s="1">
+        <v>239</v>
+      </c>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1">
+        <v>226</v>
+      </c>
+      <c r="H12" s="1">
+        <v>196</v>
+      </c>
+      <c r="I12" s="1">
+        <v>204</v>
+      </c>
+      <c r="J12" s="1">
+        <v>202</v>
+      </c>
+      <c r="K12" s="1">
+        <v>206</v>
+      </c>
+      <c r="L12" s="1">
+        <v>207</v>
+      </c>
+      <c r="N12" t="s">
+        <v>72</v>
+      </c>
+      <c r="O12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13">
+        <v>103</v>
+      </c>
+      <c r="D13">
+        <v>115</v>
+      </c>
+      <c r="E13">
+        <v>105</v>
+      </c>
+      <c r="G13">
+        <v>98</v>
+      </c>
+      <c r="H13">
+        <v>94</v>
+      </c>
+      <c r="I13" s="3">
+        <v>94</v>
+      </c>
+      <c r="J13">
+        <v>94</v>
+      </c>
+      <c r="K13">
+        <v>98</v>
+      </c>
+      <c r="L13">
+        <v>103</v>
+      </c>
+      <c r="N13" t="s">
+        <v>72</v>
+      </c>
+      <c r="O13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14">
+        <v>196</v>
+      </c>
+      <c r="D14">
+        <v>206</v>
+      </c>
+      <c r="E14">
+        <v>213</v>
+      </c>
+      <c r="G14">
+        <v>199</v>
+      </c>
+      <c r="H14">
+        <v>163</v>
+      </c>
+      <c r="I14" s="3">
+        <v>194</v>
+      </c>
+      <c r="J14">
+        <v>202</v>
+      </c>
+      <c r="K14">
+        <v>196</v>
+      </c>
+      <c r="L14">
+        <v>168</v>
+      </c>
+      <c r="N14" t="s">
+        <v>75</v>
+      </c>
+      <c r="O14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15">
+        <v>101</v>
+      </c>
+      <c r="D15">
+        <v>89</v>
+      </c>
+      <c r="E15">
+        <v>100</v>
+      </c>
+      <c r="G15">
+        <v>87</v>
+      </c>
+      <c r="H15">
+        <v>67</v>
+      </c>
+      <c r="I15" s="3">
+        <v>79</v>
+      </c>
+      <c r="J15">
+        <v>92</v>
+      </c>
+      <c r="K15">
+        <v>89</v>
+      </c>
+      <c r="L15">
+        <v>93</v>
+      </c>
+      <c r="N15" t="s">
+        <v>78</v>
+      </c>
+      <c r="O15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>77</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16">
+        <v>194</v>
+      </c>
+      <c r="D16">
+        <v>202</v>
+      </c>
+      <c r="E16">
+        <v>192</v>
+      </c>
+      <c r="G16">
+        <v>180</v>
+      </c>
+      <c r="H16">
+        <v>134</v>
+      </c>
+      <c r="I16" s="3">
+        <v>159</v>
+      </c>
+      <c r="J16">
+        <v>164</v>
+      </c>
+      <c r="K16">
+        <v>170</v>
+      </c>
+      <c r="L16">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17">
+        <v>86</v>
+      </c>
+      <c r="D17">
+        <v>94</v>
+      </c>
+      <c r="E17">
+        <v>89</v>
+      </c>
+      <c r="G17">
+        <v>89</v>
+      </c>
+      <c r="H17">
+        <v>66</v>
+      </c>
+      <c r="I17" s="3">
+        <v>73</v>
+      </c>
+      <c r="J17">
+        <v>71</v>
+      </c>
+      <c r="K17">
+        <v>78</v>
+      </c>
+      <c r="L17">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18">
+        <v>173</v>
+      </c>
+      <c r="D18">
+        <v>164</v>
+      </c>
+      <c r="E18">
+        <v>169</v>
+      </c>
+      <c r="G18">
+        <v>156</v>
+      </c>
+      <c r="H18">
+        <v>131</v>
+      </c>
+      <c r="I18" s="3">
+        <v>131</v>
+      </c>
+      <c r="J18">
+        <v>143</v>
+      </c>
+      <c r="K18">
+        <v>149</v>
+      </c>
+      <c r="L18">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+      <c r="G19">
+        <v>4</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19" s="3">
+        <v>2</v>
+      </c>
+      <c r="J19">
+        <v>4</v>
+      </c>
+      <c r="K19">
+        <v>1</v>
+      </c>
+      <c r="L19">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A1:A5 A7:A1048576">
+    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G14 A8:L8">
+    <cfRule type="duplicateValues" dxfId="2" priority="8"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A2A54E4-64DA-4F77-89C1-E605C9E6A879}">
+  <dimension ref="A1:O19"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N20" sqref="N20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2">
+        <v>2013</v>
+      </c>
+      <c r="D2" s="2">
+        <v>2014</v>
+      </c>
+      <c r="E2" s="2">
+        <v>2015</v>
+      </c>
+      <c r="F2" s="2">
+        <v>2016</v>
+      </c>
+      <c r="G2" s="2">
+        <v>2017</v>
+      </c>
+      <c r="H2" s="2">
+        <v>2018</v>
+      </c>
+      <c r="I2" s="2">
+        <v>2019</v>
+      </c>
+      <c r="J2" s="2">
+        <v>2020</v>
+      </c>
+      <c r="K2" s="2">
+        <v>2021</v>
+      </c>
+      <c r="L2" s="2">
+        <v>2022</v>
+      </c>
+      <c r="O2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="1">
+        <v>28</v>
+      </c>
+      <c r="D3" s="1">
+        <v>27</v>
+      </c>
+      <c r="E3" s="1">
+        <v>24</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1">
+        <v>21</v>
+      </c>
+      <c r="H3" s="1">
+        <v>17</v>
+      </c>
+      <c r="I3" s="1">
+        <v>19</v>
+      </c>
+      <c r="J3" s="1">
+        <v>18</v>
+      </c>
+      <c r="K3" s="1">
+        <v>20</v>
+      </c>
+      <c r="L3" s="1">
+        <v>20</v>
+      </c>
+      <c r="O3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="1">
+        <v>48</v>
+      </c>
+      <c r="D4" s="1">
+        <v>51</v>
+      </c>
+      <c r="E4" s="1">
+        <v>47</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1">
+        <v>52</v>
+      </c>
+      <c r="H4" s="1">
+        <v>39</v>
+      </c>
+      <c r="I4" s="1">
+        <v>43</v>
+      </c>
+      <c r="J4" s="1">
+        <v>42</v>
+      </c>
+      <c r="K4" s="1">
+        <v>47</v>
+      </c>
+      <c r="L4" s="1">
+        <v>37</v>
+      </c>
+      <c r="N4" t="s">
+        <v>56</v>
+      </c>
+      <c r="O4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="1">
+        <v>60</v>
+      </c>
+      <c r="D5" s="1">
+        <v>72</v>
+      </c>
+      <c r="E5" s="1">
+        <v>54</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1">
+        <v>66</v>
+      </c>
+      <c r="H5" s="1">
+        <v>45</v>
+      </c>
+      <c r="I5" s="1">
+        <v>48</v>
+      </c>
+      <c r="J5" s="1">
+        <v>49</v>
+      </c>
+      <c r="K5" s="1">
+        <v>55</v>
+      </c>
+      <c r="L5" s="1">
+        <v>49</v>
+      </c>
+      <c r="N5" t="s">
+        <v>57</v>
+      </c>
+      <c r="O5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="1">
+        <v>25</v>
+      </c>
+      <c r="D6" s="1">
+        <v>34</v>
+      </c>
+      <c r="E6" s="1">
+        <v>39</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1">
+        <v>34</v>
+      </c>
+      <c r="H6" s="1">
+        <v>29</v>
+      </c>
+      <c r="I6" s="1">
+        <v>28</v>
+      </c>
+      <c r="J6" s="1">
+        <v>34</v>
+      </c>
+      <c r="K6" s="1">
+        <v>48</v>
+      </c>
+      <c r="L6" s="1">
+        <v>37</v>
+      </c>
+      <c r="N6" t="s">
+        <v>60</v>
+      </c>
+      <c r="O6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="1">
+        <v>115</v>
+      </c>
+      <c r="D7" s="1">
+        <v>104</v>
+      </c>
+      <c r="E7" s="1">
+        <v>115</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1">
+        <v>119</v>
+      </c>
+      <c r="H7" s="1">
+        <v>95</v>
+      </c>
+      <c r="I7" s="1">
+        <v>99</v>
+      </c>
+      <c r="J7" s="1">
+        <v>98</v>
+      </c>
+      <c r="K7" s="1">
+        <v>88</v>
+      </c>
+      <c r="L7" s="1">
+        <v>78</v>
+      </c>
+      <c r="N7" t="s">
+        <v>62</v>
+      </c>
+      <c r="O7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="1">
+        <v>52</v>
+      </c>
+      <c r="D8" s="1">
+        <v>42</v>
+      </c>
+      <c r="E8" s="1">
+        <v>37</v>
+      </c>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1">
+        <v>38</v>
+      </c>
+      <c r="H8" s="1">
+        <v>25</v>
+      </c>
+      <c r="I8" s="1">
+        <v>34</v>
+      </c>
+      <c r="J8" s="1">
+        <v>35</v>
+      </c>
+      <c r="K8" s="1">
+        <v>32</v>
+      </c>
+      <c r="L8" s="1">
+        <v>39</v>
+      </c>
+      <c r="N8" t="s">
+        <v>64</v>
+      </c>
+      <c r="O8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="1">
+        <v>70</v>
+      </c>
+      <c r="D9" s="1">
+        <v>60</v>
+      </c>
+      <c r="E9" s="1">
+        <v>63</v>
+      </c>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1">
+        <v>51</v>
+      </c>
+      <c r="H9" s="1">
+        <v>46</v>
+      </c>
+      <c r="I9" s="1">
+        <v>53</v>
+      </c>
+      <c r="J9" s="1">
+        <v>46</v>
+      </c>
+      <c r="K9" s="1">
+        <v>51</v>
+      </c>
+      <c r="L9" s="1">
+        <v>66</v>
+      </c>
+      <c r="N9" t="s">
+        <v>66</v>
+      </c>
+      <c r="O9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="1">
+        <v>98</v>
+      </c>
+      <c r="D10" s="1">
+        <v>92</v>
+      </c>
+      <c r="E10" s="1">
+        <v>104</v>
+      </c>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1">
+        <v>22</v>
+      </c>
+      <c r="H10" s="1">
+        <v>81</v>
+      </c>
+      <c r="I10" s="1">
+        <v>77</v>
+      </c>
+      <c r="J10" s="1">
+        <v>87</v>
+      </c>
+      <c r="K10" s="1">
+        <v>101</v>
+      </c>
+      <c r="L10" s="1">
+        <v>87</v>
+      </c>
+      <c r="N10" t="s">
+        <v>68</v>
+      </c>
+      <c r="O10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="1">
+        <v>172</v>
+      </c>
+      <c r="D11" s="1">
+        <v>179</v>
+      </c>
+      <c r="E11" s="1">
+        <v>192</v>
+      </c>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1">
+        <v>182</v>
+      </c>
+      <c r="H11" s="1">
+        <v>154</v>
+      </c>
+      <c r="I11" s="1">
+        <v>212</v>
+      </c>
+      <c r="J11" s="1">
+        <v>173</v>
+      </c>
+      <c r="K11" s="1">
+        <v>172</v>
+      </c>
+      <c r="L11" s="1">
+        <v>167</v>
+      </c>
+      <c r="N11" t="s">
+        <v>70</v>
+      </c>
+      <c r="O11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="1">
+        <v>233</v>
+      </c>
+      <c r="D12" s="1">
+        <v>229</v>
+      </c>
+      <c r="E12" s="1">
+        <v>239</v>
+      </c>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1">
+        <v>226</v>
+      </c>
+      <c r="H12" s="1">
+        <v>196</v>
+      </c>
+      <c r="I12" s="1">
+        <v>204</v>
+      </c>
+      <c r="J12" s="1">
+        <v>202</v>
+      </c>
+      <c r="K12" s="1">
+        <v>206</v>
+      </c>
+      <c r="L12" s="1">
+        <v>207</v>
+      </c>
+      <c r="N12" t="s">
+        <v>72</v>
+      </c>
+      <c r="O12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="1">
+        <v>103</v>
+      </c>
+      <c r="D13" s="1">
+        <v>115</v>
+      </c>
+      <c r="E13" s="1">
+        <v>105</v>
+      </c>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1">
+        <v>98</v>
+      </c>
+      <c r="H13" s="1">
+        <v>94</v>
+      </c>
+      <c r="I13" s="4">
+        <v>94</v>
+      </c>
+      <c r="J13" s="1">
+        <v>94</v>
+      </c>
+      <c r="K13" s="1">
+        <v>98</v>
+      </c>
+      <c r="L13" s="1">
+        <v>103</v>
+      </c>
+      <c r="N13" t="s">
+        <v>72</v>
+      </c>
+      <c r="O13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="1">
+        <v>196</v>
+      </c>
+      <c r="D14" s="1">
+        <v>206</v>
+      </c>
+      <c r="E14" s="1">
+        <v>213</v>
+      </c>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1">
+        <v>199</v>
+      </c>
+      <c r="H14" s="1">
+        <v>163</v>
+      </c>
+      <c r="I14" s="4">
+        <v>194</v>
+      </c>
+      <c r="J14" s="1">
+        <v>202</v>
+      </c>
+      <c r="K14" s="1">
+        <v>196</v>
+      </c>
+      <c r="L14" s="1">
+        <v>168</v>
+      </c>
+      <c r="N14" t="s">
+        <v>75</v>
+      </c>
+      <c r="O14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="1">
+        <v>101</v>
+      </c>
+      <c r="D15" s="1">
+        <v>89</v>
+      </c>
+      <c r="E15" s="1">
+        <v>100</v>
+      </c>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1">
+        <v>87</v>
+      </c>
+      <c r="H15" s="1">
+        <v>67</v>
+      </c>
+      <c r="I15" s="4">
+        <v>79</v>
+      </c>
+      <c r="J15" s="1">
+        <v>92</v>
+      </c>
+      <c r="K15" s="1">
+        <v>89</v>
+      </c>
+      <c r="L15" s="1">
+        <v>93</v>
+      </c>
+      <c r="N15" t="s">
+        <v>78</v>
+      </c>
+      <c r="O15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="1">
+        <v>194</v>
+      </c>
+      <c r="D16" s="1">
+        <v>202</v>
+      </c>
+      <c r="E16" s="1">
+        <v>192</v>
+      </c>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1">
+        <v>180</v>
+      </c>
+      <c r="H16" s="1">
+        <v>134</v>
+      </c>
+      <c r="I16" s="4">
+        <v>159</v>
+      </c>
+      <c r="J16" s="1">
+        <v>164</v>
+      </c>
+      <c r="K16" s="1">
+        <v>170</v>
+      </c>
+      <c r="L16" s="1">
+        <v>155</v>
+      </c>
+      <c r="N16" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="1">
+        <v>86</v>
+      </c>
+      <c r="D17" s="1">
+        <v>94</v>
+      </c>
+      <c r="E17" s="1">
+        <v>89</v>
+      </c>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1">
+        <v>89</v>
+      </c>
+      <c r="H17" s="1">
+        <v>66</v>
+      </c>
+      <c r="I17" s="4">
+        <v>73</v>
+      </c>
+      <c r="J17" s="1">
+        <v>71</v>
+      </c>
+      <c r="K17" s="1">
+        <v>78</v>
+      </c>
+      <c r="L17" s="1">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="1">
+        <v>173</v>
+      </c>
+      <c r="D18" s="1">
+        <v>164</v>
+      </c>
+      <c r="E18" s="1">
+        <v>169</v>
+      </c>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1">
+        <v>156</v>
+      </c>
+      <c r="H18" s="1">
+        <v>131</v>
+      </c>
+      <c r="I18" s="4">
+        <v>131</v>
+      </c>
+      <c r="J18" s="1">
+        <v>143</v>
+      </c>
+      <c r="K18" s="1">
+        <v>149</v>
+      </c>
+      <c r="L18" s="1">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="1">
+        <v>2</v>
+      </c>
+      <c r="D19" s="1">
+        <v>1</v>
+      </c>
+      <c r="E19" s="1">
+        <v>2</v>
+      </c>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1">
+        <v>4</v>
+      </c>
+      <c r="H19" s="1">
+        <v>1</v>
+      </c>
+      <c r="I19" s="4">
+        <v>2</v>
+      </c>
+      <c r="J19" s="1">
+        <v>4</v>
+      </c>
+      <c r="K19" s="1">
+        <v>1</v>
+      </c>
+      <c r="L19" s="1">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A1:A5 A7:A19">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G14 A8:L8">
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>